<commit_message>
Added some additional signals documentation
</commit_message>
<xml_diff>
--- a/cnc control cabinet bom.xlsx
+++ b/cnc control cabinet bom.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="182">
   <si>
     <t>Line Reactor</t>
   </si>
@@ -523,6 +523,60 @@
   </si>
   <si>
     <t>Terminal Blocks</t>
+  </si>
+  <si>
+    <t>CYCLE_START</t>
+  </si>
+  <si>
+    <t>CNC Cycle Start</t>
+  </si>
+  <si>
+    <t>FEED_OVER</t>
+  </si>
+  <si>
+    <t>Analog</t>
+  </si>
+  <si>
+    <t>RAPID_OVER</t>
+  </si>
+  <si>
+    <t>Rapid Speed Override</t>
+  </si>
+  <si>
+    <t>Feed Speed Override</t>
+  </si>
+  <si>
+    <t>SPINDLE_ENC</t>
+  </si>
+  <si>
+    <t>Spindle Encoder</t>
+  </si>
+  <si>
+    <t>MUX</t>
+  </si>
+  <si>
+    <t>ALARM_Z</t>
+  </si>
+  <si>
+    <t>ALARM_X</t>
+  </si>
+  <si>
+    <t>ALARM_Y</t>
+  </si>
+  <si>
+    <t>Drive Alarm X-Axis</t>
+  </si>
+  <si>
+    <t>Drive Alarm Y-Axis</t>
+  </si>
+  <si>
+    <t>Drive Alarm Z-Axis</t>
+  </si>
+  <si>
+    <t>PENDANT</t>
+  </si>
+  <si>
+    <t>Motion Pendant</t>
   </si>
 </sst>
 </file>
@@ -952,12 +1006,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F21"/>
+  <dimension ref="B1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="1">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
@@ -1253,6 +1309,106 @@
       </c>
       <c r="F21" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" t="s">
+        <v>144</v>
+      </c>
+      <c r="F22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" t="s">
+        <v>170</v>
+      </c>
+      <c r="E23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" t="s">
+        <v>172</v>
+      </c>
+      <c r="E25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" t="s">
+        <v>178</v>
+      </c>
+      <c r="E27" t="s">
+        <v>144</v>
+      </c>
+      <c r="F27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D28" t="s">
+        <v>179</v>
+      </c>
+      <c r="E28" t="s">
+        <v>144</v>
+      </c>
+      <c r="F28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" t="s">
+        <v>181</v>
+      </c>
+      <c r="E29" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>